<commit_message>
Tue May 24 12:20:03 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/练习题.xlsx
+++ b/笔记/CISSP/练习题.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
   <si>
     <t>章节</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>A、B</t>
+  </si>
+  <si>
+    <t>A、B、D</t>
+  </si>
+  <si>
+    <t>A,D</t>
+  </si>
+  <si>
+    <t>A,B,D</t>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +241,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,144 +569,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,7 +714,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -704,6 +728,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1030,10 +1060,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C161" sqref="C161:D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -1291,9 +1323,1588 @@
       </c>
       <c r="E21" s="3"/>
     </row>
+    <row r="22" customHeight="1" spans="1:5">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" customHeight="1" spans="1:5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" customHeight="1" spans="1:5">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customHeight="1" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" customHeight="1" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3">
+        <v>7</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" customHeight="1" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" customHeight="1" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customHeight="1" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customHeight="1" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3">
+        <v>11</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customHeight="1" spans="1:5">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3">
+        <v>12</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customHeight="1" spans="1:5">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3">
+        <v>13</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" customHeight="1" spans="1:5">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3">
+        <v>14</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" customHeight="1" spans="1:5">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3">
+        <v>15</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" customHeight="1" spans="1:5">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" customHeight="1" spans="1:5">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3">
+        <v>17</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" customHeight="1" spans="1:5">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3">
+        <v>18</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" customHeight="1" spans="1:5">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3">
+        <v>19</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" customHeight="1" spans="1:5">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3">
+        <v>20</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" customHeight="1" spans="1:5">
+      <c r="A42" s="3">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" customHeight="1" spans="1:5">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" customHeight="1" spans="1:5">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3">
+        <v>3</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" customHeight="1" spans="1:5">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3">
+        <v>4</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" customHeight="1" spans="1:5">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" customHeight="1" spans="1:5">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3">
+        <v>6</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3">
+        <v>7</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" customHeight="1" spans="1:5">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3">
+        <v>8</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" customHeight="1" spans="1:5">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3">
+        <v>9</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" customHeight="1" spans="1:5">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3">
+        <v>10</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" customHeight="1" spans="1:5">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3">
+        <v>11</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" customHeight="1" spans="1:5">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3">
+        <v>12</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" customHeight="1" spans="1:5">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3">
+        <v>13</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" customHeight="1" spans="1:5">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3">
+        <v>14</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" customHeight="1" spans="1:5">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3">
+        <v>15</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" customHeight="1" spans="1:5">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3">
+        <v>16</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" customHeight="1" spans="1:5">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3">
+        <v>17</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" customHeight="1" spans="1:5">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3">
+        <v>18</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" customHeight="1" spans="1:5">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3">
+        <v>19</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" customHeight="1" spans="1:5">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3">
+        <v>20</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" customHeight="1" spans="1:5">
+      <c r="A62" s="3">
+        <v>8</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" customHeight="1" spans="1:5">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3">
+        <v>2</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" customHeight="1" spans="1:5">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3">
+        <v>3</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" customHeight="1" spans="1:5">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3">
+        <v>4</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" customHeight="1" spans="1:5">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3">
+        <v>5</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" customHeight="1" spans="1:5">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3">
+        <v>6</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" customHeight="1" spans="1:5">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3">
+        <v>7</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" customHeight="1" spans="1:5">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3">
+        <v>8</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" customHeight="1" spans="1:5">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3">
+        <v>9</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" customHeight="1" spans="1:5">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3">
+        <v>10</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" customHeight="1" spans="1:5">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3">
+        <v>11</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" customHeight="1" spans="1:5">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3">
+        <v>12</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" customHeight="1" spans="1:5">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3">
+        <v>13</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" customHeight="1" spans="1:5">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3">
+        <v>14</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" customHeight="1" spans="1:5">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3">
+        <v>15</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" customHeight="1" spans="1:5">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3">
+        <v>16</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" customHeight="1" spans="1:5">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3">
+        <v>17</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" customHeight="1" spans="1:5">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3">
+        <v>18</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" customHeight="1" spans="1:5">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3">
+        <v>19</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" customHeight="1" spans="1:5">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3">
+        <v>20</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" customHeight="1" spans="1:5">
+      <c r="A82" s="3">
+        <v>9</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" customHeight="1" spans="1:5">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3">
+        <v>2</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" customHeight="1" spans="1:5">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3">
+        <v>3</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" customHeight="1" spans="1:5">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3">
+        <v>4</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" customHeight="1" spans="1:5">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3">
+        <v>5</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" customHeight="1" spans="1:5">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3">
+        <v>6</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" customHeight="1" spans="1:5">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3">
+        <v>7</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" customHeight="1" spans="1:5">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3">
+        <v>8</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" customHeight="1" spans="1:5">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3">
+        <v>9</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" customHeight="1" spans="1:5">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3">
+        <v>10</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" customHeight="1" spans="1:5">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3">
+        <v>11</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" customHeight="1" spans="1:5">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3">
+        <v>12</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" customHeight="1" spans="1:5">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3">
+        <v>13</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" customHeight="1" spans="1:5">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3">
+        <v>14</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" customHeight="1" spans="1:5">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3">
+        <v>15</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" customHeight="1" spans="1:5">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3">
+        <v>16</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" customHeight="1" spans="1:5">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3">
+        <v>17</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" customHeight="1" spans="1:5">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3">
+        <v>18</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" customHeight="1" spans="1:5">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3">
+        <v>19</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" customHeight="1" spans="1:5">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3">
+        <v>20</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" customHeight="1" spans="1:5">
+      <c r="A102" s="3">
+        <v>10</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" customHeight="1" spans="1:5">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3">
+        <v>2</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" customHeight="1" spans="1:5">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3">
+        <v>3</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" customHeight="1" spans="1:5">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3">
+        <v>4</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" customHeight="1" spans="1:5">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3">
+        <v>5</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" customHeight="1" spans="1:5">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3">
+        <v>6</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" customHeight="1" spans="1:5">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3">
+        <v>7</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" customHeight="1" spans="1:5">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3">
+        <v>8</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" customHeight="1" spans="1:5">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3">
+        <v>9</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" customHeight="1" spans="1:5">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3">
+        <v>10</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" customHeight="1" spans="1:5">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3">
+        <v>11</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" customHeight="1" spans="1:5">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3">
+        <v>12</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" customHeight="1" spans="1:5">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3">
+        <v>13</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" customHeight="1" spans="1:5">
+      <c r="A115" s="3"/>
+      <c r="B115" s="3">
+        <v>14</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" customHeight="1" spans="1:5">
+      <c r="A116" s="3"/>
+      <c r="B116" s="3">
+        <v>15</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" customHeight="1" spans="1:5">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3">
+        <v>16</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" customHeight="1" spans="1:5">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3">
+        <v>17</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" customHeight="1" spans="1:5">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3">
+        <v>18</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" customHeight="1" spans="1:5">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3">
+        <v>19</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" customHeight="1" spans="1:5">
+      <c r="A121" s="3"/>
+      <c r="B121" s="3">
+        <v>20</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" customHeight="1" spans="1:5">
+      <c r="A122" s="3">
+        <v>11</v>
+      </c>
+      <c r="B122" s="3">
+        <v>1</v>
+      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" customHeight="1" spans="1:5">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" customHeight="1" spans="1:5">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3">
+        <v>3</v>
+      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" customHeight="1" spans="1:5">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3">
+        <v>4</v>
+      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" customHeight="1" spans="1:5">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3">
+        <v>5</v>
+      </c>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" customHeight="1" spans="1:5">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3">
+        <v>6</v>
+      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" customHeight="1" spans="1:5">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3">
+        <v>7</v>
+      </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" customHeight="1" spans="1:5">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3">
+        <v>8</v>
+      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+    </row>
+    <row r="130" customHeight="1" spans="1:5">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3">
+        <v>9</v>
+      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" customHeight="1" spans="1:5">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3">
+        <v>10</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" customHeight="1" spans="1:5">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3">
+        <v>11</v>
+      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" customHeight="1" spans="1:5">
+      <c r="A133" s="3"/>
+      <c r="B133" s="3">
+        <v>12</v>
+      </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+    </row>
+    <row r="134" customHeight="1" spans="1:5">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3">
+        <v>13</v>
+      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" customHeight="1" spans="1:5">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3">
+        <v>14</v>
+      </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" customHeight="1" spans="1:5">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3">
+        <v>15</v>
+      </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" customHeight="1" spans="1:5">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3">
+        <v>16</v>
+      </c>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" customHeight="1" spans="1:5">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3">
+        <v>17</v>
+      </c>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" customHeight="1" spans="1:5">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3">
+        <v>18</v>
+      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" customHeight="1" spans="1:5">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3">
+        <v>19</v>
+      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" customHeight="1" spans="1:5">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3">
+        <v>20</v>
+      </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+    </row>
+    <row r="142" customHeight="1" spans="1:5">
+      <c r="A142" s="3">
+        <v>12</v>
+      </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" customHeight="1" spans="1:5">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3">
+        <v>2</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+    </row>
+    <row r="144" customHeight="1" spans="1:5">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3">
+        <v>3</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+    </row>
+    <row r="145" customHeight="1" spans="1:5">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3">
+        <v>4</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+    </row>
+    <row r="146" customHeight="1" spans="1:5">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3">
+        <v>5</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+    </row>
+    <row r="147" customHeight="1" spans="1:5">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3">
+        <v>6</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+    </row>
+    <row r="148" customHeight="1" spans="1:5">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3">
+        <v>7</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E148" s="3"/>
+    </row>
+    <row r="149" customHeight="1" spans="1:5">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3">
+        <v>8</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+    </row>
+    <row r="150" customHeight="1" spans="1:5">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3">
+        <v>9</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+    </row>
+    <row r="151" customHeight="1" spans="1:5">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3">
+        <v>10</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
+    </row>
+    <row r="152" customHeight="1" spans="1:5">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3">
+        <v>11</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+    </row>
+    <row r="153" customHeight="1" spans="1:5">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3">
+        <v>12</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" customHeight="1" spans="1:5">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3">
+        <v>13</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" customHeight="1" spans="1:5">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3">
+        <v>14</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" customHeight="1" spans="1:5">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3">
+        <v>15</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" customHeight="1" spans="1:5">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3">
+        <v>16</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+    </row>
+    <row r="158" customHeight="1" spans="1:5">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3">
+        <v>17</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+    </row>
+    <row r="159" customHeight="1" spans="1:5">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3">
+        <v>18</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
+    </row>
+    <row r="160" customHeight="1" spans="1:5">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3">
+        <v>19</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" customHeight="1" spans="1:5">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3">
+        <v>20</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E161" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
     <mergeCell ref="A2:A21"/>
+    <mergeCell ref="A22:A41"/>
+    <mergeCell ref="A42:A61"/>
+    <mergeCell ref="A62:A81"/>
+    <mergeCell ref="A82:A101"/>
+    <mergeCell ref="A102:A121"/>
+    <mergeCell ref="A122:A141"/>
+    <mergeCell ref="A142:A161"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Mon May 30 00:29:25 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/练习题.xlsx
+++ b/笔记/CISSP/练习题.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
   <si>
     <t>章节</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>A,B,D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>矩阵中每一个文件都有一个单独的ACL(访问控制列表)</t>
+  </si>
+  <si>
+    <t>开放，关闭，过滤</t>
+  </si>
+  <si>
+    <t>A,B,C</t>
+  </si>
+  <si>
+    <t>社区与部署模型为两个或更多个组织提供云资产</t>
   </si>
 </sst>
 </file>
@@ -443,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -461,6 +476,43 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -599,7 +651,7 @@
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -641,10 +693,10 @@
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -653,28 +705,28 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -695,13 +747,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -714,27 +766,36 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1060,12 +1121,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C161" sqref="C161:D161"/>
+      <selection pane="bottomLeft" activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -1074,7 +1135,7 @@
     <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.84375" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.046875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2895,8 +2956,930 @@
       </c>
       <c r="E161" s="3"/>
     </row>
+    <row r="162" customHeight="1" spans="1:5">
+      <c r="A162" s="3">
+        <v>13</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" s="6"/>
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" customHeight="1" spans="1:5">
+      <c r="A163" s="3"/>
+      <c r="B163" s="3">
+        <v>2</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+    </row>
+    <row r="164" customHeight="1" spans="1:5">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3">
+        <v>3</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+    </row>
+    <row r="165" customHeight="1" spans="1:5">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3">
+        <v>4</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" s="3"/>
+      <c r="E165" s="3"/>
+    </row>
+    <row r="166" customHeight="1" spans="1:5">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3">
+        <v>5</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+    </row>
+    <row r="167" customHeight="1" spans="1:5">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3">
+        <v>6</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="3"/>
+      <c r="E167" s="3"/>
+    </row>
+    <row r="168" customHeight="1" spans="1:5">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3">
+        <v>7</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E168" s="3"/>
+    </row>
+    <row r="169" customHeight="1" spans="1:5">
+      <c r="A169" s="3"/>
+      <c r="B169" s="3">
+        <v>8</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+    </row>
+    <row r="170" customHeight="1" spans="1:5">
+      <c r="A170" s="3"/>
+      <c r="B170" s="3">
+        <v>9</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+    </row>
+    <row r="171" customHeight="1" spans="1:5">
+      <c r="A171" s="3"/>
+      <c r="B171" s="3">
+        <v>10</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E171" s="3"/>
+    </row>
+    <row r="172" customHeight="1" spans="1:5">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3">
+        <v>11</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D172" s="3"/>
+      <c r="E172" s="3"/>
+    </row>
+    <row r="173" customHeight="1" spans="1:5">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3">
+        <v>12</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+    </row>
+    <row r="174" customHeight="1" spans="1:5">
+      <c r="A174" s="3"/>
+      <c r="B174" s="3">
+        <v>13</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" s="3"/>
+    </row>
+    <row r="175" customHeight="1" spans="1:5">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3">
+        <v>14</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D175" s="3"/>
+      <c r="E175" s="3"/>
+    </row>
+    <row r="176" customHeight="1" spans="1:5">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3">
+        <v>15</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+    </row>
+    <row r="177" customHeight="1" spans="1:5">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3">
+        <v>16</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="3"/>
+      <c r="E177" s="3"/>
+    </row>
+    <row r="178" customHeight="1" spans="1:5">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3">
+        <v>17</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E178" s="3"/>
+    </row>
+    <row r="179" customHeight="1" spans="1:5">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3">
+        <v>18</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" s="3"/>
+      <c r="E179" s="3"/>
+    </row>
+    <row r="180" customHeight="1" spans="1:5">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3">
+        <v>19</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+    </row>
+    <row r="181" customHeight="1" spans="1:5">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3">
+        <v>20</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181" s="3"/>
+      <c r="E181" s="3"/>
+    </row>
+    <row r="182" customHeight="1" spans="1:5">
+      <c r="A182" s="7">
+        <v>14</v>
+      </c>
+      <c r="B182" s="3">
+        <v>1</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+    </row>
+    <row r="183" customHeight="1" spans="1:5">
+      <c r="A183" s="8"/>
+      <c r="B183" s="3">
+        <v>2</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="3"/>
+    </row>
+    <row r="184" customHeight="1" spans="1:5">
+      <c r="A184" s="8"/>
+      <c r="B184" s="3">
+        <v>3</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="185" customHeight="1" spans="1:5">
+      <c r="A185" s="8"/>
+      <c r="B185" s="3">
+        <v>4</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+    </row>
+    <row r="186" customHeight="1" spans="1:5">
+      <c r="A186" s="8"/>
+      <c r="B186" s="3">
+        <v>5</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E186" s="3"/>
+    </row>
+    <row r="187" customHeight="1" spans="1:5">
+      <c r="A187" s="8"/>
+      <c r="B187" s="3">
+        <v>6</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+    </row>
+    <row r="188" customHeight="1" spans="1:5">
+      <c r="A188" s="8"/>
+      <c r="B188" s="3">
+        <v>7</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+    </row>
+    <row r="189" customHeight="1" spans="1:5">
+      <c r="A189" s="8"/>
+      <c r="B189" s="3">
+        <v>8</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E189" s="3"/>
+    </row>
+    <row r="190" customHeight="1" spans="1:5">
+      <c r="A190" s="8"/>
+      <c r="B190" s="3">
+        <v>9</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+    </row>
+    <row r="191" customHeight="1" spans="1:5">
+      <c r="A191" s="8"/>
+      <c r="B191" s="3">
+        <v>10</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+    </row>
+    <row r="192" customHeight="1" spans="1:5">
+      <c r="A192" s="8"/>
+      <c r="B192" s="3">
+        <v>11</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+    </row>
+    <row r="193" customHeight="1" spans="1:5">
+      <c r="A193" s="8"/>
+      <c r="B193" s="3">
+        <v>12</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
+    </row>
+    <row r="194" customHeight="1" spans="1:5">
+      <c r="A194" s="8"/>
+      <c r="B194" s="3">
+        <v>13</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
+    </row>
+    <row r="195" customHeight="1" spans="1:5">
+      <c r="A195" s="8"/>
+      <c r="B195" s="3">
+        <v>14</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+    </row>
+    <row r="196" customHeight="1" spans="1:5">
+      <c r="A196" s="8"/>
+      <c r="B196" s="3">
+        <v>15</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+    </row>
+    <row r="197" customHeight="1" spans="1:5">
+      <c r="A197" s="8"/>
+      <c r="B197" s="3">
+        <v>16</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E197" s="3"/>
+    </row>
+    <row r="198" customHeight="1" spans="1:5">
+      <c r="A198" s="8"/>
+      <c r="B198" s="3">
+        <v>17</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+    </row>
+    <row r="199" customHeight="1" spans="1:5">
+      <c r="A199" s="8"/>
+      <c r="B199" s="3">
+        <v>18</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" s="3"/>
+      <c r="E199" s="3"/>
+    </row>
+    <row r="200" customHeight="1" spans="1:5">
+      <c r="A200" s="8"/>
+      <c r="B200" s="3">
+        <v>19</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+    </row>
+    <row r="201" customHeight="1" spans="1:5">
+      <c r="A201" s="9"/>
+      <c r="B201" s="3">
+        <v>20</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+    </row>
+    <row r="202" customHeight="1" spans="1:5">
+      <c r="A202" s="3">
+        <v>15</v>
+      </c>
+      <c r="B202" s="3">
+        <v>1</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+    </row>
+    <row r="203" customHeight="1" spans="1:5">
+      <c r="A203" s="3"/>
+      <c r="B203" s="3">
+        <v>2</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="204" customHeight="1" spans="1:5">
+      <c r="A204" s="3"/>
+      <c r="B204" s="3">
+        <v>3</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+    </row>
+    <row r="205" customHeight="1" spans="1:5">
+      <c r="A205" s="3"/>
+      <c r="B205" s="3">
+        <v>4</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+    </row>
+    <row r="206" customHeight="1" spans="1:5">
+      <c r="A206" s="3"/>
+      <c r="B206" s="3">
+        <v>5</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+    </row>
+    <row r="207" customHeight="1" spans="1:5">
+      <c r="A207" s="3"/>
+      <c r="B207" s="3">
+        <v>6</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E207" s="3"/>
+    </row>
+    <row r="208" customHeight="1" spans="1:5">
+      <c r="A208" s="3"/>
+      <c r="B208" s="3">
+        <v>7</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" s="3"/>
+      <c r="E208" s="3"/>
+    </row>
+    <row r="209" customHeight="1" spans="1:5">
+      <c r="A209" s="3"/>
+      <c r="B209" s="3">
+        <v>8</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" s="3"/>
+      <c r="E209" s="3"/>
+    </row>
+    <row r="210" customHeight="1" spans="1:5">
+      <c r="A210" s="3"/>
+      <c r="B210" s="3">
+        <v>9</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+    </row>
+    <row r="211" customHeight="1" spans="1:5">
+      <c r="A211" s="3"/>
+      <c r="B211" s="3">
+        <v>10</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D211" s="3"/>
+      <c r="E211" s="3"/>
+    </row>
+    <row r="212" customHeight="1" spans="1:5">
+      <c r="A212" s="3"/>
+      <c r="B212" s="3">
+        <v>11</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" s="3"/>
+      <c r="E212" s="3"/>
+    </row>
+    <row r="213" customHeight="1" spans="1:5">
+      <c r="A213" s="3"/>
+      <c r="B213" s="3">
+        <v>12</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="3"/>
+      <c r="E213" s="3"/>
+    </row>
+    <row r="214" customHeight="1" spans="1:5">
+      <c r="A214" s="3"/>
+      <c r="B214" s="3">
+        <v>13</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D214" s="3"/>
+      <c r="E214" s="3"/>
+    </row>
+    <row r="215" customHeight="1" spans="1:5">
+      <c r="A215" s="3"/>
+      <c r="B215" s="3">
+        <v>14</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+    </row>
+    <row r="216" customHeight="1" spans="1:5">
+      <c r="A216" s="3"/>
+      <c r="B216" s="3">
+        <v>15</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D216" s="3"/>
+      <c r="E216" s="3"/>
+    </row>
+    <row r="217" customHeight="1" spans="1:5">
+      <c r="A217" s="3"/>
+      <c r="B217" s="3">
+        <v>16</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+    </row>
+    <row r="218" customHeight="1" spans="1:5">
+      <c r="A218" s="3"/>
+      <c r="B218" s="3">
+        <v>17</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D218" s="3"/>
+      <c r="E218" s="3"/>
+    </row>
+    <row r="219" customHeight="1" spans="1:5">
+      <c r="A219" s="3"/>
+      <c r="B219" s="3">
+        <v>18</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D219" s="3"/>
+      <c r="E219" s="3"/>
+    </row>
+    <row r="220" customHeight="1" spans="1:5">
+      <c r="A220" s="3"/>
+      <c r="B220" s="3">
+        <v>19</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" s="3"/>
+    </row>
+    <row r="221" customHeight="1" spans="1:5">
+      <c r="A221" s="3"/>
+      <c r="B221" s="3">
+        <v>20</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+    </row>
+    <row r="222" customHeight="1" spans="1:5">
+      <c r="A222" s="3">
+        <v>16</v>
+      </c>
+      <c r="B222" s="3">
+        <v>1</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+    </row>
+    <row r="223" customHeight="1" spans="1:5">
+      <c r="A223" s="3"/>
+      <c r="B223" s="3">
+        <v>2</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+    </row>
+    <row r="224" customHeight="1" spans="1:5">
+      <c r="A224" s="3"/>
+      <c r="B224" s="3">
+        <v>3</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D224" s="3"/>
+      <c r="E224" s="3"/>
+    </row>
+    <row r="225" customHeight="1" spans="1:5">
+      <c r="A225" s="3"/>
+      <c r="B225" s="3">
+        <v>4</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D225" s="3"/>
+      <c r="E225" s="3"/>
+    </row>
+    <row r="226" customHeight="1" spans="1:5">
+      <c r="A226" s="3"/>
+      <c r="B226" s="3">
+        <v>5</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+    </row>
+    <row r="227" customHeight="1" spans="1:5">
+      <c r="A227" s="3"/>
+      <c r="B227" s="3">
+        <v>6</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D227" s="3"/>
+      <c r="E227" s="3"/>
+    </row>
+    <row r="228" customHeight="1" spans="1:5">
+      <c r="A228" s="3"/>
+      <c r="B228" s="3">
+        <v>7</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D228" s="3"/>
+      <c r="E228" s="3"/>
+    </row>
+    <row r="229" customHeight="1" spans="1:5">
+      <c r="A229" s="3"/>
+      <c r="B229" s="3">
+        <v>8</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D229" s="3"/>
+      <c r="E229" s="3"/>
+    </row>
+    <row r="230" customHeight="1" spans="1:5">
+      <c r="A230" s="3"/>
+      <c r="B230" s="3">
+        <v>9</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D230" s="3"/>
+      <c r="E230" s="3"/>
+    </row>
+    <row r="231" customHeight="1" spans="1:5">
+      <c r="A231" s="3"/>
+      <c r="B231" s="3">
+        <v>10</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D231" s="3"/>
+      <c r="E231" s="3"/>
+    </row>
+    <row r="232" customHeight="1" spans="1:5">
+      <c r="A232" s="3"/>
+      <c r="B232" s="3">
+        <v>11</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D232" s="3"/>
+      <c r="E232" s="3"/>
+    </row>
+    <row r="233" customHeight="1" spans="1:5">
+      <c r="A233" s="3"/>
+      <c r="B233" s="3">
+        <v>12</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+    </row>
+    <row r="234" customHeight="1" spans="1:5">
+      <c r="A234" s="3"/>
+      <c r="B234" s="3">
+        <v>13</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
+    </row>
+    <row r="235" customHeight="1" spans="1:5">
+      <c r="A235" s="3"/>
+      <c r="B235" s="3">
+        <v>14</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="236" customHeight="1" spans="1:5">
+      <c r="A236" s="3"/>
+      <c r="B236" s="3">
+        <v>15</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+    </row>
+    <row r="237" customHeight="1" spans="1:5">
+      <c r="A237" s="3"/>
+      <c r="B237" s="3">
+        <v>16</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+    </row>
+    <row r="238" customHeight="1" spans="1:5">
+      <c r="A238" s="3"/>
+      <c r="B238" s="3">
+        <v>17</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+    </row>
+    <row r="239" customHeight="1" spans="1:5">
+      <c r="A239" s="3"/>
+      <c r="B239" s="3">
+        <v>18</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D239" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E239" s="3"/>
+    </row>
+    <row r="240" customHeight="1" spans="1:5">
+      <c r="A240" s="3"/>
+      <c r="B240" s="3">
+        <v>19</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
+    </row>
+    <row r="241" customHeight="1" spans="1:5">
+      <c r="A241" s="3"/>
+      <c r="B241" s="3">
+        <v>20</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D241" s="3"/>
+      <c r="E241" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A22:A41"/>
     <mergeCell ref="A42:A61"/>
@@ -2905,6 +3888,10 @@
     <mergeCell ref="A102:A121"/>
     <mergeCell ref="A122:A141"/>
     <mergeCell ref="A142:A161"/>
+    <mergeCell ref="A162:A181"/>
+    <mergeCell ref="A182:A201"/>
+    <mergeCell ref="A202:A221"/>
+    <mergeCell ref="A222:A241"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>